<commit_message>
Adding comments into the files
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BillingAddress.xlsx
+++ b/src/test/resources/testdata/BillingAddress.xlsx
@@ -42,19 +42,19 @@
     <t>phone</t>
   </si>
   <si>
-    <t>venu</t>
-  </si>
-  <si>
-    <t>sonu</t>
-  </si>
-  <si>
-    <t>v21@gmail.com</t>
-  </si>
-  <si>
-    <t>new york</t>
-  </si>
-  <si>
-    <t>435-jshdfg</t>
+    <t>Kollapudi</t>
+  </si>
+  <si>
+    <t>Venu</t>
+  </si>
+  <si>
+    <t>venukollapudi@gmail.com</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>william Street</t>
   </si>
 </sst>
 </file>
@@ -386,10 +386,13 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -431,10 +434,10 @@
         <v>11</v>
       </c>
       <c r="F2">
-        <v>45789</v>
+        <v>10001</v>
       </c>
       <c r="G2">
-        <v>78964521</v>
+        <v>7013606690</v>
       </c>
     </row>
   </sheetData>

</xml_diff>